<commit_message>
feat: added some new params in code
</commit_message>
<xml_diff>
--- a/resultados_rdr2.xlsx
+++ b/resultados_rdr2.xlsx
@@ -10,6 +10,7 @@
     <sheet name="10000" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="100000" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="100000000" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="1000000000" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -459,10 +460,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3349</v>
+        <v>3500</v>
       </c>
       <c r="C2" t="n">
-        <v>33.48999999999999</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
@@ -472,10 +473,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>590</v>
+        <v>531</v>
       </c>
       <c r="C3" t="n">
-        <v>5.899999999999999</v>
+        <v>5.31</v>
       </c>
     </row>
     <row r="4">
@@ -485,10 +486,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2147</v>
+        <v>2110</v>
       </c>
       <c r="C4" t="n">
-        <v>21.47</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="5">
@@ -498,10 +499,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3914</v>
+        <v>3859</v>
       </c>
       <c r="C5" t="n">
-        <v>39.14</v>
+        <v>38.59</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +512,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>28.33</v>
+        <v>52.7</v>
       </c>
     </row>
   </sheetData>
@@ -557,10 +558,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>33809</v>
+        <v>33976</v>
       </c>
       <c r="C2" t="n">
-        <v>33.809</v>
+        <v>33.976</v>
       </c>
     </row>
     <row r="3">
@@ -570,10 +571,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5931</v>
+        <v>6110</v>
       </c>
       <c r="C3" t="n">
-        <v>5.931</v>
+        <v>6.11</v>
       </c>
     </row>
     <row r="4">
@@ -583,10 +584,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>21213</v>
+        <v>20817</v>
       </c>
       <c r="C4" t="n">
-        <v>21.213</v>
+        <v>20.817</v>
       </c>
     </row>
     <row r="5">
@@ -596,10 +597,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>39047</v>
+        <v>39097</v>
       </c>
       <c r="C5" t="n">
-        <v>39.047</v>
+        <v>39.097</v>
       </c>
     </row>
     <row r="6">
@@ -609,7 +610,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>27.94</v>
+        <v>51.86</v>
       </c>
     </row>
   </sheetData>
@@ -655,10 +656,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>34006267</v>
+        <v>34006624</v>
       </c>
       <c r="C2" t="n">
-        <v>34.006267</v>
+        <v>34.006624</v>
       </c>
     </row>
     <row r="3">
@@ -668,10 +669,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5999566</v>
+        <v>6000263</v>
       </c>
       <c r="C3" t="n">
-        <v>5.999566</v>
+        <v>6.000263</v>
       </c>
     </row>
     <row r="4">
@@ -681,10 +682,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>20999193</v>
+        <v>21003694</v>
       </c>
       <c r="C4" t="n">
-        <v>20.999193</v>
+        <v>21.003694</v>
       </c>
     </row>
     <row r="5">
@@ -694,10 +695,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>38994974</v>
+        <v>38989419</v>
       </c>
       <c r="C5" t="n">
-        <v>38.994974</v>
+        <v>38.989419</v>
       </c>
     </row>
     <row r="6">
@@ -706,9 +707,107 @@
           <t>Cutscene do Cavalo</t>
         </is>
       </c>
+      <c r="C6" t="n">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Ocorrências</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Probabilidade</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Final A</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>339996378</v>
+      </c>
+      <c r="C2" t="n">
+        <v>33.9996378</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Final B</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>60004236</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6.0004236</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Final C</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>209975093</v>
+      </c>
+      <c r="C4" t="n">
+        <v>20.9975093</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Final D</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>390024293</v>
+      </c>
+      <c r="C5" t="n">
+        <v>39.0024293</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cutscene do Cavalo</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>28</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>